<commit_message>
Refactor: move and rename quant model modules
Moved and renamed quant model and component modules to a new signals/quant_models/ directory structure for improved organization. Updated import paths and fixed references accordingly. Also removed obsolete LSTM unit tests and made minor config import corrections in components.
</commit_message>
<xml_diff>
--- a/CHECK LIST.xlsx
+++ b/CHECK LIST.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NGUYEN QUANG THANG\complex-trading-crypto-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A180A9E-A558-421C-B789-43D2EB11DCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F906F9DA-D091-4449-A1DF-612F6CAFE002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11640" yWindow="-4305" windowWidth="11760" windowHeight="20010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PEP8" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="74">
   <si>
     <t>signals_transformer.py</t>
   </si>
@@ -255,6 +256,9 @@
   </si>
   <si>
     <t>BỔ SUNG TESTCASE</t>
+  </si>
+  <si>
+    <t>trading_signal_analyzer.py  9.67/10 - update logger (OLD)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +292,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +323,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -401,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -440,6 +450,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -1422,4 +1434,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED6F0D0-95B0-4B5E-93F0-15A8B7D8AAF0}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>